<commit_message>
topic_2 updtes on equity
</commit_message>
<xml_diff>
--- a/topic_2_img/Topic 2 Sol.xlsx
+++ b/topic_2_img/Topic 2 Sol.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="54">
   <si>
     <t xml:space="preserve">Case 1: Borrowing $1,000,000 from a bank at a 5% interest rate:</t>
   </si>
@@ -545,7 +545,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -800,8 +800,8 @@
   </sheetPr>
   <dimension ref="B2:M116"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A94" colorId="64" zoomScale="134" zoomScaleNormal="134" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I108" activeCellId="0" sqref="I108"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A102" colorId="64" zoomScale="134" zoomScaleNormal="134" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G123" activeCellId="0" sqref="G123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1066,7 +1066,7 @@
         <v>2</v>
       </c>
       <c r="C33" s="4" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1762,8 +1762,13 @@
         <f aca="false">+J89</f>
         <v>-100000</v>
       </c>
-      <c r="L100" s="10"/>
-      <c r="M100" s="11"/>
+      <c r="L100" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="M100" s="11" t="n">
+        <f aca="false">+E97</f>
+        <v>-50000</v>
+      </c>
     </row>
     <row r="101" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D101" s="10"/>
@@ -1813,8 +1818,6 @@
       <c r="B106" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="J106" s="0"/>
-      <c r="L106" s="0"/>
     </row>
     <row r="107" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="2"/>
@@ -1830,8 +1833,6 @@
       <c r="I107" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="J107" s="0"/>
-      <c r="L107" s="0"/>
     </row>
     <row r="108" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="2"/>
@@ -1896,7 +1897,6 @@
       <c r="F112" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="I112" s="0"/>
     </row>
     <row r="113" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H113" s="32"/>
@@ -1911,10 +1911,10 @@
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H114" s="0" t="s">
+      <c r="H114" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I114" s="0" t="n">
+      <c r="I114" s="1" t="n">
         <f aca="false">I109/I108</f>
         <v>0.8</v>
       </c>

</xml_diff>

<commit_message>
topic 2 excel minor correction
</commit_message>
<xml_diff>
--- a/topic_2_img/Topic 2 Sol.xlsx
+++ b/topic_2_img/Topic 2 Sol.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Data/Github/lecture_financial_statements_analysis/topic_2_img/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E66E6B-EAA0-0644-A8CA-620F708F90AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D18FCDF-6813-5443-AD3B-55FBC24524FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="22540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1_loan" sheetId="1" r:id="rId1"/>
@@ -462,7 +462,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -494,13 +494,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -764,7 +767,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:M119"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A46" zoomScale="176" zoomScaleNormal="176" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A30" zoomScale="176" zoomScaleNormal="176" workbookViewId="0">
       <selection activeCell="B119" sqref="B119"/>
     </sheetView>
   </sheetViews>
@@ -805,20 +808,20 @@
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="I9" s="31" t="s">
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="I9" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="J9" s="31"/>
-      <c r="L9" s="31" t="s">
+      <c r="J9" s="32"/>
+      <c r="L9" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="M9" s="31"/>
+      <c r="M9" s="32"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D10" s="5" t="s">
@@ -911,20 +914,20 @@
       </c>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="D20" s="31" t="s">
+      <c r="D20" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="I20" s="31" t="s">
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="I20" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="J20" s="31"/>
-      <c r="L20" s="31" t="s">
+      <c r="J20" s="32"/>
+      <c r="L20" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="M20" s="31"/>
+      <c r="M20" s="32"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D21" s="5" t="s">
@@ -1047,20 +1050,20 @@
     </row>
     <row r="36" spans="2:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.15"/>
     <row r="37" spans="2:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.15">
-      <c r="D37" s="32" t="s">
+      <c r="D37" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="E37" s="32"/>
-      <c r="F37" s="32"/>
-      <c r="G37" s="32"/>
-      <c r="I37" s="32" t="s">
+      <c r="E37" s="33"/>
+      <c r="F37" s="33"/>
+      <c r="G37" s="33"/>
+      <c r="I37" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="J37" s="32"/>
-      <c r="L37" s="32" t="s">
+      <c r="J37" s="33"/>
+      <c r="L37" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="M37" s="32"/>
+      <c r="M37" s="33"/>
     </row>
     <row r="38" spans="2:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="D38" s="16" t="s">
@@ -1161,20 +1164,20 @@
       </c>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="D45" s="31" t="s">
+      <c r="D45" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="E45" s="31"/>
-      <c r="F45" s="31"/>
-      <c r="G45" s="31"/>
-      <c r="I45" s="31" t="s">
+      <c r="E45" s="32"/>
+      <c r="F45" s="32"/>
+      <c r="G45" s="32"/>
+      <c r="I45" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="J45" s="31"/>
-      <c r="L45" s="31" t="s">
+      <c r="J45" s="32"/>
+      <c r="L45" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="M45" s="31"/>
+      <c r="M45" s="32"/>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D46" s="5" t="s">
@@ -1302,20 +1305,20 @@
     </row>
     <row r="60" spans="2:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.15"/>
     <row r="61" spans="2:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.15">
-      <c r="D61" s="32" t="s">
+      <c r="D61" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="E61" s="32"/>
-      <c r="F61" s="32"/>
-      <c r="G61" s="32"/>
-      <c r="I61" s="32" t="s">
+      <c r="E61" s="33"/>
+      <c r="F61" s="33"/>
+      <c r="G61" s="33"/>
+      <c r="I61" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="J61" s="32"/>
-      <c r="L61" s="32" t="s">
+      <c r="J61" s="33"/>
+      <c r="L61" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="M61" s="32"/>
+      <c r="M61" s="33"/>
     </row>
     <row r="62" spans="2:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="D62" s="16" t="s">
@@ -1419,20 +1422,20 @@
     </row>
     <row r="71" spans="2:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.15"/>
     <row r="72" spans="2:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.15">
-      <c r="D72" s="31" t="s">
+      <c r="D72" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="E72" s="31"/>
-      <c r="F72" s="31"/>
-      <c r="G72" s="31"/>
-      <c r="I72" s="31" t="s">
+      <c r="E72" s="32"/>
+      <c r="F72" s="32"/>
+      <c r="G72" s="32"/>
+      <c r="I72" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="J72" s="31"/>
-      <c r="L72" s="31" t="s">
+      <c r="J72" s="32"/>
+      <c r="L72" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="M72" s="31"/>
+      <c r="M72" s="32"/>
     </row>
     <row r="73" spans="2:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="D73" s="5" t="s">
@@ -1547,20 +1550,20 @@
     </row>
     <row r="83" spans="2:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.15"/>
     <row r="84" spans="2:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.15">
-      <c r="D84" s="31" t="s">
+      <c r="D84" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="E84" s="31"/>
-      <c r="F84" s="31"/>
-      <c r="G84" s="31"/>
-      <c r="I84" s="31" t="s">
+      <c r="E84" s="32"/>
+      <c r="F84" s="32"/>
+      <c r="G84" s="32"/>
+      <c r="I84" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="J84" s="31"/>
-      <c r="L84" s="31" t="s">
+      <c r="J84" s="32"/>
+      <c r="L84" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="M84" s="31"/>
+      <c r="M84" s="32"/>
     </row>
     <row r="85" spans="2:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="D85" s="5" t="s">
@@ -1657,20 +1660,20 @@
       </c>
     </row>
     <row r="95" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="D95" s="31" t="s">
+      <c r="D95" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="E95" s="31"/>
-      <c r="F95" s="31"/>
-      <c r="G95" s="31"/>
-      <c r="I95" s="31" t="s">
+      <c r="E95" s="32"/>
+      <c r="F95" s="32"/>
+      <c r="G95" s="32"/>
+      <c r="I95" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="J95" s="31"/>
-      <c r="L95" s="31" t="s">
+      <c r="J95" s="32"/>
+      <c r="L95" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="M95" s="31"/>
+      <c r="M95" s="32"/>
     </row>
     <row r="96" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D96" s="5" t="s">
@@ -1810,7 +1813,7 @@
       <c r="D107" t="s">
         <v>35</v>
       </c>
-      <c r="F107" s="33" t="s">
+      <c r="F107" s="31" t="s">
         <v>36</v>
       </c>
       <c r="I107" t="s">
@@ -1825,7 +1828,7 @@
       <c r="D108" t="s">
         <v>35</v>
       </c>
-      <c r="F108" s="33" t="s">
+      <c r="F108" s="31" t="s">
         <v>36</v>
       </c>
       <c r="H108" t="s">
@@ -1851,7 +1854,7 @@
       <c r="C110" t="s">
         <v>42</v>
       </c>
-      <c r="D110" s="33" t="s">
+      <c r="D110" s="31" t="s">
         <v>36</v>
       </c>
       <c r="F110" t="s">
@@ -1868,14 +1871,14 @@
       <c r="B111" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D111" s="33"/>
+      <c r="D111" s="31"/>
     </row>
     <row r="112" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B112" s="1"/>
       <c r="C112" t="s">
         <v>45</v>
       </c>
-      <c r="D112" s="33" t="s">
+      <c r="D112" s="31" t="s">
         <v>36</v>
       </c>
       <c r="F112" t="s">
@@ -1933,30 +1936,30 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="D84:G84"/>
+    <mergeCell ref="I84:J84"/>
+    <mergeCell ref="L84:M84"/>
+    <mergeCell ref="D95:G95"/>
+    <mergeCell ref="I95:J95"/>
+    <mergeCell ref="L95:M95"/>
+    <mergeCell ref="D61:G61"/>
+    <mergeCell ref="I61:J61"/>
+    <mergeCell ref="L61:M61"/>
+    <mergeCell ref="D72:G72"/>
+    <mergeCell ref="I72:J72"/>
+    <mergeCell ref="L72:M72"/>
+    <mergeCell ref="D37:G37"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="L37:M37"/>
+    <mergeCell ref="D45:G45"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="L45:M45"/>
     <mergeCell ref="D9:G9"/>
     <mergeCell ref="I9:J9"/>
     <mergeCell ref="L9:M9"/>
     <mergeCell ref="D20:G20"/>
     <mergeCell ref="I20:J20"/>
     <mergeCell ref="L20:M20"/>
-    <mergeCell ref="D37:G37"/>
-    <mergeCell ref="I37:J37"/>
-    <mergeCell ref="L37:M37"/>
-    <mergeCell ref="D45:G45"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="L45:M45"/>
-    <mergeCell ref="D61:G61"/>
-    <mergeCell ref="I61:J61"/>
-    <mergeCell ref="L61:M61"/>
-    <mergeCell ref="D72:G72"/>
-    <mergeCell ref="I72:J72"/>
-    <mergeCell ref="L72:M72"/>
-    <mergeCell ref="D84:G84"/>
-    <mergeCell ref="I84:J84"/>
-    <mergeCell ref="L84:M84"/>
-    <mergeCell ref="D95:G95"/>
-    <mergeCell ref="I95:J95"/>
-    <mergeCell ref="L95:M95"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1971,8 +1974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:M27"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="176" zoomScaleNormal="176" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15:M15"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="176" zoomScaleNormal="176" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1991,20 +1994,20 @@
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="I4" s="31" t="s">
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="I4" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="31"/>
-      <c r="L4" s="31" t="s">
+      <c r="J4" s="32"/>
+      <c r="L4" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="31"/>
+      <c r="M4" s="32"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D5" s="5" t="s">
@@ -2098,26 +2101,27 @@
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="D15" s="31" t="s">
+      <c r="D15" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="I15" s="31" t="s">
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="I15" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="J15" s="31"/>
-      <c r="L15" s="31" t="s">
+      <c r="J15" s="32"/>
+      <c r="L15" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="M15" s="31"/>
+      <c r="M15" s="32"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D16" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="E16" s="34"/>
+      <c r="F16" s="35" t="s">
         <v>7</v>
       </c>
       <c r="G16" s="7"/>
@@ -2134,10 +2138,10 @@
       <c r="D17" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="36">
         <v>-300000</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="34" t="s">
         <v>53</v>
       </c>
       <c r="G17" s="9">
@@ -2145,10 +2149,13 @@
       </c>
       <c r="I17" s="8"/>
       <c r="J17" s="9"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="7"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D18" s="8"/>
-      <c r="E18" s="2"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="34"/>
       <c r="G18" s="7"/>
       <c r="I18" s="8"/>
       <c r="J18" s="9"/>
@@ -2157,8 +2164,8 @@
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D19" s="8"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="6" t="s">
+      <c r="E19" s="36"/>
+      <c r="F19" s="35" t="s">
         <v>12</v>
       </c>
       <c r="G19" s="7"/>
@@ -2173,7 +2180,9 @@
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D20" s="8"/>
-      <c r="E20" s="2"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="7"/>
       <c r="I20" s="8"/>
       <c r="J20" s="9"/>
       <c r="L20" s="8" t="s">

</xml_diff>